<commit_message>
Good parameter set for ponton convex cost
</commit_message>
<xml_diff>
--- a/flat_NLP_previous/stats.xlsx
+++ b/flat_NLP_previous/stats.xlsx
@@ -579,82 +579,82 @@
         <v>4</v>
       </c>
       <c r="H4">
-        <v>7.57331</v>
+        <v>15.02477</v>
       </c>
       <c r="I4">
-        <v>7.8001</v>
+        <v>15.538</v>
       </c>
       <c r="M4" t="s">
         <v>4</v>
       </c>
       <c r="N4">
-        <v>11.47977</v>
+        <v>27.12381</v>
       </c>
       <c r="O4">
-        <v>11.721</v>
+        <v>27.612</v>
       </c>
       <c r="S4" t="s">
         <v>4</v>
       </c>
       <c r="T4">
-        <v>32.13317</v>
+        <v>14.63619</v>
       </c>
       <c r="U4">
-        <v>32.349</v>
+        <v>15.122</v>
       </c>
       <c r="Y4" t="s">
         <v>4</v>
       </c>
       <c r="Z4">
-        <v>45.44727</v>
+        <v>27.38689</v>
       </c>
       <c r="AA4">
-        <v>45.702</v>
+        <v>27.792</v>
       </c>
       <c r="AE4" t="s">
         <v>4</v>
       </c>
       <c r="AF4">
-        <v>35.23465</v>
+        <v>39.9933</v>
       </c>
       <c r="AG4">
-        <v>35.45</v>
+        <v>40.43</v>
       </c>
       <c r="AK4" t="s">
         <v>4</v>
       </c>
       <c r="AL4">
-        <v>44.49975</v>
+        <v>34.6543</v>
       </c>
       <c r="AM4">
-        <v>44.701</v>
+        <v>35.086</v>
       </c>
       <c r="AQ4" t="s">
         <v>4</v>
       </c>
       <c r="AR4">
-        <v>38.27976</v>
+        <v>58.12295</v>
       </c>
       <c r="AS4">
-        <v>38.52</v>
+        <v>58.509</v>
       </c>
       <c r="AW4" t="s">
         <v>4</v>
       </c>
       <c r="AX4">
-        <v>39.3774</v>
+        <v>29.72335</v>
       </c>
       <c r="AY4">
-        <v>39.59</v>
+        <v>30.151</v>
       </c>
       <c r="BC4" t="s">
         <v>4</v>
       </c>
       <c r="BD4">
-        <v>67.1767</v>
+        <v>44.20329</v>
       </c>
       <c r="BE4">
-        <v>67.351</v>
+        <v>44.594</v>
       </c>
     </row>
     <row r="5" spans="7:57">
@@ -662,82 +662,82 @@
         <v>5</v>
       </c>
       <c r="H5">
-        <v>2.23966</v>
+        <v>0.90916</v>
       </c>
       <c r="I5">
-        <v>2.4608</v>
+        <v>1.1637</v>
       </c>
       <c r="M5" t="s">
         <v>5</v>
       </c>
       <c r="N5">
-        <v>1.51763</v>
+        <v>2.0048</v>
       </c>
       <c r="O5">
-        <v>1.7682</v>
+        <v>2.2515</v>
       </c>
       <c r="S5" t="s">
         <v>5</v>
       </c>
       <c r="T5">
-        <v>6.29398</v>
+        <v>4.67097</v>
       </c>
       <c r="U5">
-        <v>6.4766</v>
+        <v>4.9134</v>
       </c>
       <c r="Y5" t="s">
         <v>5</v>
       </c>
       <c r="Z5">
-        <v>11.84147</v>
+        <v>4.17268</v>
       </c>
       <c r="AA5">
-        <v>12.091</v>
+        <v>4.4214</v>
       </c>
       <c r="AE5" t="s">
         <v>5</v>
       </c>
       <c r="AF5">
-        <v>20.47144</v>
+        <v>9.571479999999999</v>
       </c>
       <c r="AG5">
-        <v>20.682</v>
+        <v>9.8184</v>
       </c>
       <c r="AK5" t="s">
         <v>5</v>
       </c>
       <c r="AL5">
-        <v>19.18037</v>
+        <v>15.82747</v>
       </c>
       <c r="AM5">
-        <v>19.38</v>
+        <v>16.071</v>
       </c>
       <c r="AQ5" t="s">
         <v>5</v>
       </c>
       <c r="AR5">
-        <v>9.18464</v>
+        <v>13.59377</v>
       </c>
       <c r="AS5">
-        <v>9.417999999999999</v>
+        <v>13.792</v>
       </c>
       <c r="AW5" t="s">
         <v>5</v>
       </c>
       <c r="AX5">
-        <v>23.00161</v>
+        <v>3.61694</v>
       </c>
       <c r="AY5">
-        <v>23.218</v>
+        <v>3.8263</v>
       </c>
       <c r="BC5" t="s">
         <v>5</v>
       </c>
       <c r="BD5">
-        <v>23.19091</v>
+        <v>17.21639</v>
       </c>
       <c r="BE5">
-        <v>23.42</v>
+        <v>17.434</v>
       </c>
     </row>
     <row r="6" spans="7:57">
@@ -745,82 +745,82 @@
         <v>6</v>
       </c>
       <c r="H6">
-        <v>0.6747300000000001</v>
+        <v>0.5255</v>
       </c>
       <c r="I6">
-        <v>0.9137</v>
+        <v>0.7664</v>
       </c>
       <c r="M6" t="s">
         <v>6</v>
       </c>
       <c r="N6">
-        <v>0.68415</v>
+        <v>0.82516</v>
       </c>
       <c r="O6">
-        <v>0.9083</v>
+        <v>1.0615</v>
       </c>
       <c r="S6" t="s">
         <v>6</v>
       </c>
       <c r="T6">
-        <v>1.32774</v>
+        <v>1.11215</v>
       </c>
       <c r="U6">
-        <v>1.5691</v>
+        <v>1.3615</v>
       </c>
       <c r="Y6" t="s">
         <v>6</v>
       </c>
       <c r="Z6">
-        <v>1.27423</v>
+        <v>1.80948</v>
       </c>
       <c r="AA6">
-        <v>1.5073</v>
+        <v>2.0582</v>
       </c>
       <c r="AE6" t="s">
         <v>6</v>
       </c>
       <c r="AF6">
-        <v>2.67845</v>
+        <v>2.00077</v>
       </c>
       <c r="AG6">
-        <v>2.9084</v>
+        <v>2.2479</v>
       </c>
       <c r="AK6" t="s">
         <v>6</v>
       </c>
       <c r="AL6">
-        <v>1.61566</v>
+        <v>1.65881</v>
       </c>
       <c r="AM6">
-        <v>1.8232</v>
+        <v>1.8669</v>
       </c>
       <c r="AQ6" t="s">
         <v>6</v>
       </c>
       <c r="AR6">
-        <v>2.10279</v>
+        <v>2.40802</v>
       </c>
       <c r="AS6">
-        <v>2.3299</v>
+        <v>2.608</v>
       </c>
       <c r="AW6" t="s">
         <v>6</v>
       </c>
       <c r="AX6">
-        <v>2.31459</v>
+        <v>2.02528</v>
       </c>
       <c r="AY6">
-        <v>2.4617</v>
+        <v>2.2647</v>
       </c>
       <c r="BC6" t="s">
         <v>6</v>
       </c>
       <c r="BD6">
-        <v>2.90587</v>
+        <v>2.78609</v>
       </c>
       <c r="BE6">
-        <v>3.081</v>
+        <v>3.0282</v>
       </c>
     </row>
     <row r="7" spans="7:57">
@@ -828,82 +828,82 @@
         <v>7</v>
       </c>
       <c r="H7">
-        <v>1.66574</v>
+        <v>1.5977</v>
       </c>
       <c r="I7">
-        <v>1.9143</v>
+        <v>1.8362</v>
       </c>
       <c r="M7" t="s">
         <v>7</v>
       </c>
       <c r="N7">
-        <v>1.91935</v>
+        <v>10.24865</v>
       </c>
       <c r="O7">
-        <v>2.157</v>
+        <v>10.482</v>
       </c>
       <c r="S7" t="s">
         <v>7</v>
       </c>
       <c r="T7">
-        <v>1.35211</v>
+        <v>1.42762</v>
       </c>
       <c r="U7">
-        <v>1.594</v>
+        <v>1.6775</v>
       </c>
       <c r="Y7" t="s">
         <v>7</v>
       </c>
       <c r="Z7">
-        <v>1.1946</v>
+        <v>1.87332</v>
       </c>
       <c r="AA7">
-        <v>1.4153</v>
+        <v>2.0946</v>
       </c>
       <c r="AE7" t="s">
         <v>7</v>
       </c>
       <c r="AF7">
-        <v>1.36253</v>
+        <v>3.87217</v>
       </c>
       <c r="AG7">
-        <v>1.5984</v>
+        <v>4.1192</v>
       </c>
       <c r="AK7" t="s">
         <v>7</v>
       </c>
       <c r="AL7">
-        <v>1.58613</v>
+        <v>5.60397</v>
       </c>
       <c r="AM7">
-        <v>1.7882</v>
+        <v>5.8148</v>
       </c>
       <c r="AQ7" t="s">
         <v>7</v>
       </c>
       <c r="AR7">
-        <v>1.69104</v>
+        <v>1.60306</v>
       </c>
       <c r="AS7">
-        <v>1.9208</v>
+        <v>1.8016</v>
       </c>
       <c r="AW7" t="s">
         <v>7</v>
       </c>
       <c r="AX7">
-        <v>2.37235</v>
+        <v>1.96629</v>
       </c>
       <c r="AY7">
-        <v>2.6107</v>
+        <v>2.2073</v>
       </c>
       <c r="BC7" t="s">
         <v>7</v>
       </c>
       <c r="BD7">
-        <v>1.90376</v>
+        <v>2.29399</v>
       </c>
       <c r="BE7">
-        <v>2.1438</v>
+        <v>2.5294</v>
       </c>
     </row>
     <row r="8" spans="7:57">
@@ -911,82 +911,82 @@
         <v>8</v>
       </c>
       <c r="H8">
-        <v>0.979</v>
+        <v>0.49821</v>
       </c>
       <c r="I8">
-        <v>1.2254</v>
+        <v>0.7228</v>
       </c>
       <c r="M8" t="s">
         <v>8</v>
       </c>
       <c r="N8">
-        <v>1.5598</v>
+        <v>1.17455</v>
       </c>
       <c r="O8">
-        <v>1.7949</v>
+        <v>1.4263</v>
       </c>
       <c r="S8" t="s">
         <v>8</v>
       </c>
       <c r="T8">
-        <v>1.49432</v>
+        <v>1.19417</v>
       </c>
       <c r="U8">
-        <v>1.7459</v>
+        <v>1.445</v>
       </c>
       <c r="Y8" t="s">
         <v>8</v>
       </c>
       <c r="Z8">
-        <v>2.83635</v>
+        <v>2.64418</v>
       </c>
       <c r="AA8">
-        <v>3.0579</v>
+        <v>2.8681</v>
       </c>
       <c r="AE8" t="s">
         <v>8</v>
       </c>
       <c r="AF8">
-        <v>1.55771</v>
+        <v>1.39196</v>
       </c>
       <c r="AG8">
-        <v>1.7578</v>
+        <v>1.6392</v>
       </c>
       <c r="AK8" t="s">
         <v>8</v>
       </c>
       <c r="AL8">
-        <v>1.95133</v>
+        <v>2.06034</v>
       </c>
       <c r="AM8">
-        <v>2.1652</v>
+        <v>2.2705</v>
       </c>
       <c r="AQ8" t="s">
         <v>8</v>
       </c>
       <c r="AR8">
-        <v>1.75937</v>
+        <v>2.37274</v>
       </c>
       <c r="AS8">
-        <v>1.9635</v>
+        <v>2.6145</v>
       </c>
       <c r="AW8" t="s">
         <v>8</v>
       </c>
       <c r="AX8">
-        <v>2.14247</v>
+        <v>1.97004</v>
       </c>
       <c r="AY8">
-        <v>2.3661</v>
+        <v>2.2117</v>
       </c>
       <c r="BC8" t="s">
         <v>8</v>
       </c>
       <c r="BD8">
-        <v>2.67602</v>
+        <v>4.02666</v>
       </c>
       <c r="BE8">
-        <v>2.8529</v>
+        <v>4.2378</v>
       </c>
     </row>
     <row r="9" spans="7:57">
@@ -994,82 +994,82 @@
         <v>9</v>
       </c>
       <c r="H9">
-        <v>1.9737</v>
+        <v>1.13173</v>
       </c>
       <c r="I9">
-        <v>2.2225</v>
+        <v>1.3859</v>
       </c>
       <c r="M9" t="s">
         <v>9</v>
       </c>
       <c r="N9">
-        <v>0.62897</v>
+        <v>0.66127</v>
       </c>
       <c r="O9">
-        <v>0.8598</v>
+        <v>0.9137</v>
       </c>
       <c r="S9" t="s">
         <v>9</v>
       </c>
       <c r="T9">
-        <v>1.51367</v>
+        <v>1.05895</v>
       </c>
       <c r="U9">
-        <v>1.744</v>
+        <v>1.3097</v>
       </c>
       <c r="Y9" t="s">
         <v>9</v>
       </c>
       <c r="Z9">
-        <v>1.38072</v>
+        <v>1.14147</v>
       </c>
       <c r="AA9">
-        <v>1.6007</v>
+        <v>1.366</v>
       </c>
       <c r="AE9" t="s">
         <v>9</v>
       </c>
       <c r="AF9">
-        <v>2.29245</v>
+        <v>1.5349</v>
       </c>
       <c r="AG9">
-        <v>2.4864</v>
+        <v>1.7821</v>
       </c>
       <c r="AK9" t="s">
         <v>9</v>
       </c>
       <c r="AL9">
-        <v>1.67424</v>
+        <v>1.4461</v>
       </c>
       <c r="AM9">
-        <v>1.8957</v>
+        <v>1.6551</v>
       </c>
       <c r="AQ9" t="s">
         <v>9</v>
       </c>
       <c r="AR9">
-        <v>2.20693</v>
+        <v>2.21852</v>
       </c>
       <c r="AS9">
-        <v>2.4433</v>
+        <v>2.4199</v>
       </c>
       <c r="AW9" t="s">
         <v>9</v>
       </c>
       <c r="AX9">
-        <v>2.14708</v>
+        <v>1.9983</v>
       </c>
       <c r="AY9">
-        <v>2.3886</v>
+        <v>2.2398</v>
       </c>
       <c r="BC9" t="s">
         <v>9</v>
       </c>
       <c r="BD9">
-        <v>2.88104</v>
+        <v>2.91527</v>
       </c>
       <c r="BE9">
-        <v>3.1172</v>
+        <v>3.1541</v>
       </c>
     </row>
     <row r="10" spans="7:57">
@@ -1077,82 +1077,82 @@
         <v>10</v>
       </c>
       <c r="H10">
-        <v>0.83691</v>
+        <v>0.40154</v>
       </c>
       <c r="I10">
-        <v>1.0857</v>
+        <v>0.6566</v>
       </c>
       <c r="M10" t="s">
         <v>10</v>
       </c>
       <c r="N10">
-        <v>0.75522</v>
+        <v>0.59634</v>
       </c>
       <c r="O10">
-        <v>0.9814000000000001</v>
+        <v>0.849</v>
       </c>
       <c r="S10" t="s">
         <v>10</v>
       </c>
       <c r="T10">
-        <v>1.48641</v>
+        <v>1.16205</v>
       </c>
       <c r="U10">
-        <v>1.71</v>
+        <v>1.413</v>
       </c>
       <c r="Y10" t="s">
         <v>10</v>
       </c>
       <c r="Z10">
-        <v>4.89043</v>
+        <v>1.49689</v>
       </c>
       <c r="AA10">
-        <v>5.1257</v>
+        <v>1.7178</v>
       </c>
       <c r="AE10" t="s">
         <v>10</v>
       </c>
       <c r="AF10">
-        <v>1.98467</v>
+        <v>1.48339</v>
       </c>
       <c r="AG10">
-        <v>2.2031</v>
+        <v>1.7305</v>
       </c>
       <c r="AK10" t="s">
         <v>10</v>
       </c>
       <c r="AL10">
-        <v>2.11607</v>
+        <v>1.44539</v>
       </c>
       <c r="AM10">
-        <v>2.3086</v>
+        <v>1.6508</v>
       </c>
       <c r="AQ10" t="s">
         <v>10</v>
       </c>
       <c r="AR10">
-        <v>2.60367</v>
+        <v>9.08253</v>
       </c>
       <c r="AS10">
-        <v>2.8407</v>
+        <v>9.2822</v>
       </c>
       <c r="AW10" t="s">
         <v>10</v>
       </c>
       <c r="AX10">
-        <v>1.71798</v>
+        <v>1.87174</v>
       </c>
       <c r="AY10">
-        <v>1.9549</v>
+        <v>2.1129</v>
       </c>
       <c r="BC10" t="s">
         <v>10</v>
       </c>
       <c r="BD10">
-        <v>2.30886</v>
+        <v>4.93135</v>
       </c>
       <c r="BE10">
-        <v>2.536</v>
+        <v>5.1688</v>
       </c>
     </row>
     <row r="11" spans="7:57">
@@ -1160,82 +1160,82 @@
         <v>11</v>
       </c>
       <c r="H11">
-        <v>1.13384</v>
+        <v>0.98989</v>
       </c>
       <c r="I11">
-        <v>1.3808</v>
+        <v>1.2454</v>
       </c>
       <c r="M11" t="s">
         <v>11</v>
       </c>
       <c r="N11">
-        <v>1.14466</v>
+        <v>0.58375</v>
       </c>
       <c r="O11">
-        <v>1.379</v>
+        <v>0.8342000000000001</v>
       </c>
       <c r="S11" t="s">
         <v>11</v>
       </c>
       <c r="T11">
-        <v>1.11364</v>
+        <v>1.59103</v>
       </c>
       <c r="U11">
-        <v>1.3434</v>
+        <v>1.8417</v>
       </c>
       <c r="Y11" t="s">
         <v>11</v>
       </c>
       <c r="Z11">
-        <v>1.19312</v>
+        <v>1.53706</v>
       </c>
       <c r="AA11">
-        <v>1.4413</v>
+        <v>1.7518</v>
       </c>
       <c r="AE11" t="s">
         <v>11</v>
       </c>
       <c r="AF11">
-        <v>2.08238</v>
+        <v>1.76513</v>
       </c>
       <c r="AG11">
-        <v>2.2942</v>
+        <v>2.0115</v>
       </c>
       <c r="AK11" t="s">
         <v>11</v>
       </c>
       <c r="AL11">
-        <v>1.75276</v>
+        <v>2.11222</v>
       </c>
       <c r="AM11">
-        <v>1.9733</v>
+        <v>2.3167</v>
       </c>
       <c r="AQ11" t="s">
         <v>11</v>
       </c>
       <c r="AR11">
-        <v>1.89241</v>
+        <v>1.79684</v>
       </c>
       <c r="AS11">
-        <v>2.1372</v>
+        <v>2.0063</v>
       </c>
       <c r="AW11" t="s">
         <v>11</v>
       </c>
       <c r="AX11">
-        <v>2.26433</v>
+        <v>2.53612</v>
       </c>
       <c r="AY11">
-        <v>2.4888</v>
+        <v>2.7771</v>
       </c>
       <c r="BC11" t="s">
         <v>11</v>
       </c>
       <c r="BD11">
-        <v>2.4115</v>
+        <v>2.76634</v>
       </c>
       <c r="BE11">
-        <v>2.5991</v>
+        <v>3.0039</v>
       </c>
     </row>
     <row r="12" spans="7:57">
@@ -1243,82 +1243,82 @@
         <v>12</v>
       </c>
       <c r="H12">
-        <v>0.523</v>
+        <v>0.9222900000000001</v>
       </c>
       <c r="I12">
-        <v>0.7714</v>
+        <v>1.1292</v>
       </c>
       <c r="M12" t="s">
         <v>12</v>
       </c>
       <c r="N12">
-        <v>1.96535</v>
+        <v>1.8297</v>
       </c>
       <c r="O12">
-        <v>2.1988</v>
+        <v>2.0822</v>
       </c>
       <c r="S12" t="s">
         <v>12</v>
       </c>
       <c r="T12">
-        <v>0.87453</v>
+        <v>1.06916</v>
       </c>
       <c r="U12">
-        <v>1.1125</v>
+        <v>1.3202</v>
       </c>
       <c r="Y12" t="s">
         <v>12</v>
       </c>
       <c r="Z12">
-        <v>1.74516</v>
+        <v>3.98525</v>
       </c>
       <c r="AA12">
-        <v>1.9596</v>
+        <v>4.2015</v>
       </c>
       <c r="AE12" t="s">
         <v>12</v>
       </c>
       <c r="AF12">
-        <v>1.9061</v>
+        <v>1.42647</v>
       </c>
       <c r="AG12">
-        <v>2.1399</v>
+        <v>1.6731</v>
       </c>
       <c r="AK12" t="s">
         <v>12</v>
       </c>
       <c r="AL12">
-        <v>1.42552</v>
+        <v>1.63168</v>
       </c>
       <c r="AM12">
-        <v>1.6443</v>
+        <v>1.8404</v>
       </c>
       <c r="AQ12" t="s">
         <v>12</v>
       </c>
       <c r="AR12">
-        <v>1.89832</v>
+        <v>2.30231</v>
       </c>
       <c r="AS12">
-        <v>2.1371</v>
+        <v>2.5441</v>
       </c>
       <c r="AW12" t="s">
         <v>12</v>
       </c>
       <c r="AX12">
-        <v>2.25429</v>
+        <v>2.06305</v>
       </c>
       <c r="AY12">
-        <v>2.4581</v>
+        <v>2.256</v>
       </c>
       <c r="BC12" t="s">
         <v>12</v>
       </c>
       <c r="BD12">
-        <v>2.40298</v>
+        <v>2.37927</v>
       </c>
       <c r="BE12">
-        <v>2.5889</v>
+        <v>2.6189</v>
       </c>
     </row>
     <row r="13" spans="7:57">
@@ -1326,82 +1326,82 @@
         <v>13</v>
       </c>
       <c r="H13">
-        <v>1.09283</v>
+        <v>0.66629</v>
       </c>
       <c r="I13">
-        <v>1.3389</v>
+        <v>0.9087</v>
       </c>
       <c r="M13" t="s">
         <v>13</v>
       </c>
       <c r="N13">
-        <v>0.86399</v>
+        <v>0.5888099999999999</v>
       </c>
       <c r="O13">
-        <v>1.0899</v>
+        <v>0.8413</v>
       </c>
       <c r="S13" t="s">
         <v>13</v>
       </c>
       <c r="T13">
-        <v>1.11385</v>
+        <v>1.21667</v>
       </c>
       <c r="U13">
-        <v>1.3491</v>
+        <v>1.4676</v>
       </c>
       <c r="Y13" t="s">
         <v>13</v>
       </c>
       <c r="Z13">
-        <v>4.55484</v>
+        <v>1.39581</v>
       </c>
       <c r="AA13">
-        <v>4.7916</v>
+        <v>1.6134</v>
       </c>
       <c r="AE13" t="s">
         <v>13</v>
       </c>
       <c r="AF13">
-        <v>1.36191</v>
+        <v>1.36915</v>
       </c>
       <c r="AG13">
-        <v>1.5786</v>
+        <v>1.6159</v>
       </c>
       <c r="AK13" t="s">
         <v>13</v>
       </c>
       <c r="AL13">
-        <v>1.33191</v>
+        <v>1.40749</v>
       </c>
       <c r="AM13">
-        <v>1.5395</v>
+        <v>1.6153</v>
       </c>
       <c r="AQ13" t="s">
         <v>13</v>
       </c>
       <c r="AR13">
-        <v>1.94869</v>
+        <v>2.07805</v>
       </c>
       <c r="AS13">
-        <v>2.152</v>
+        <v>2.3193</v>
       </c>
       <c r="AW13" t="s">
         <v>13</v>
       </c>
       <c r="AX13">
-        <v>2.36828</v>
+        <v>1.7656</v>
       </c>
       <c r="AY13">
-        <v>2.607</v>
+        <v>1.9707</v>
       </c>
       <c r="BC13" t="s">
         <v>13</v>
       </c>
       <c r="BD13">
-        <v>2.24371</v>
+        <v>2.09541</v>
       </c>
       <c r="BE13">
-        <v>2.4567</v>
+        <v>2.3369</v>
       </c>
     </row>
     <row r="14" spans="7:57">
@@ -1409,82 +1409,82 @@
         <v>14</v>
       </c>
       <c r="H14">
-        <v>0.46789</v>
+        <v>0.62904</v>
       </c>
       <c r="I14">
-        <v>0.7175</v>
+        <v>0.8705000000000001</v>
       </c>
       <c r="M14" t="s">
         <v>14</v>
       </c>
       <c r="N14">
-        <v>0.98295</v>
+        <v>0.53109</v>
       </c>
       <c r="O14">
-        <v>1.2157</v>
+        <v>0.7835</v>
       </c>
       <c r="S14" t="s">
         <v>14</v>
       </c>
       <c r="T14">
-        <v>0.9883999999999999</v>
+        <v>1.00415</v>
       </c>
       <c r="U14">
-        <v>1.2293</v>
+        <v>1.255</v>
       </c>
       <c r="Y14" t="s">
         <v>14</v>
       </c>
       <c r="Z14">
-        <v>1.45763</v>
+        <v>3.89881</v>
       </c>
       <c r="AA14">
-        <v>1.6771</v>
+        <v>4.1141</v>
       </c>
       <c r="AE14" t="s">
         <v>14</v>
       </c>
       <c r="AF14">
-        <v>2.398</v>
+        <v>1.50333</v>
       </c>
       <c r="AG14">
-        <v>2.6175</v>
+        <v>1.7494</v>
       </c>
       <c r="AK14" t="s">
         <v>14</v>
       </c>
       <c r="AL14">
-        <v>1.5212</v>
+        <v>1.58531</v>
       </c>
       <c r="AM14">
-        <v>1.7437</v>
+        <v>1.7924</v>
       </c>
       <c r="AQ14" t="s">
         <v>14</v>
       </c>
       <c r="AR14">
-        <v>1.82373</v>
+        <v>2.07419</v>
       </c>
       <c r="AS14">
-        <v>2.0556</v>
+        <v>2.3159</v>
       </c>
       <c r="AW14" t="s">
         <v>14</v>
       </c>
       <c r="AX14">
-        <v>2.5695</v>
+        <v>1.971</v>
       </c>
       <c r="AY14">
-        <v>2.7628</v>
+        <v>2.2129</v>
       </c>
       <c r="BC14" t="s">
         <v>14</v>
       </c>
       <c r="BD14">
-        <v>5.2215</v>
+        <v>2.19716</v>
       </c>
       <c r="BE14">
-        <v>5.4559</v>
+        <v>2.4364</v>
       </c>
     </row>
     <row r="15" spans="7:57">
@@ -1492,82 +1492,82 @@
         <v>15</v>
       </c>
       <c r="H15">
-        <v>0.83051</v>
+        <v>1.61868</v>
       </c>
       <c r="I15">
-        <v>1.0784</v>
+        <v>1.8599</v>
       </c>
       <c r="M15" t="s">
         <v>15</v>
       </c>
       <c r="N15">
-        <v>0.73926</v>
+        <v>0.56973</v>
       </c>
       <c r="O15">
-        <v>0.9846</v>
+        <v>0.8221000000000001</v>
       </c>
       <c r="S15" t="s">
         <v>15</v>
       </c>
       <c r="T15">
-        <v>3.57433</v>
+        <v>0.99751</v>
       </c>
       <c r="U15">
-        <v>3.8065</v>
+        <v>1.2483</v>
       </c>
       <c r="Y15" t="s">
         <v>15</v>
       </c>
       <c r="Z15">
-        <v>1.12093</v>
+        <v>1.349</v>
       </c>
       <c r="AA15">
-        <v>1.339</v>
+        <v>1.5689</v>
       </c>
       <c r="AE15" t="s">
         <v>15</v>
       </c>
       <c r="AF15">
-        <v>3.77266</v>
+        <v>1.22685</v>
       </c>
       <c r="AG15">
-        <v>3.9812</v>
+        <v>1.4739</v>
       </c>
       <c r="AK15" t="s">
         <v>15</v>
       </c>
       <c r="AL15">
-        <v>1.99091</v>
+        <v>1.84049</v>
       </c>
       <c r="AM15">
-        <v>2.1983</v>
+        <v>2.0463</v>
       </c>
       <c r="AQ15" t="s">
         <v>15</v>
       </c>
       <c r="AR15">
-        <v>1.67524</v>
+        <v>2.28466</v>
       </c>
       <c r="AS15">
-        <v>1.8744</v>
+        <v>2.5255</v>
       </c>
       <c r="AW15" t="s">
         <v>15</v>
       </c>
       <c r="AX15">
-        <v>1.67038</v>
+        <v>2.65709</v>
       </c>
       <c r="AY15">
-        <v>1.9059</v>
+        <v>2.8956</v>
       </c>
       <c r="BC15" t="s">
         <v>15</v>
       </c>
       <c r="BD15">
-        <v>2.6783</v>
+        <v>3.72877</v>
       </c>
       <c r="BE15">
-        <v>2.9054</v>
+        <v>3.9685</v>
       </c>
     </row>
     <row r="16" spans="7:57">
@@ -1575,82 +1575,82 @@
         <v>16</v>
       </c>
       <c r="H16">
-        <v>0.43069</v>
+        <v>1.06575</v>
       </c>
       <c r="I16">
-        <v>0.6709000000000001</v>
+        <v>1.3064</v>
       </c>
       <c r="M16" t="s">
         <v>16</v>
       </c>
       <c r="N16">
-        <v>1.46305</v>
+        <v>0.7601</v>
       </c>
       <c r="O16">
-        <v>1.7095</v>
+        <v>1.0125</v>
       </c>
       <c r="S16" t="s">
         <v>16</v>
       </c>
       <c r="T16">
-        <v>1.08775</v>
+        <v>1.94654</v>
       </c>
       <c r="U16">
-        <v>1.3163</v>
+        <v>2.1975</v>
       </c>
       <c r="Y16" t="s">
         <v>16</v>
       </c>
       <c r="Z16">
-        <v>3.56702</v>
+        <v>1.17078</v>
       </c>
       <c r="AA16">
-        <v>3.7877</v>
+        <v>1.3929</v>
       </c>
       <c r="AE16" t="s">
         <v>16</v>
       </c>
       <c r="AF16">
-        <v>1.55515</v>
+        <v>2.12387</v>
       </c>
       <c r="AG16">
-        <v>1.7675</v>
+        <v>2.3703</v>
       </c>
       <c r="AK16" t="s">
         <v>16</v>
       </c>
       <c r="AL16">
-        <v>2.04335</v>
+        <v>1.47311</v>
       </c>
       <c r="AM16">
-        <v>2.2578</v>
+        <v>1.68</v>
       </c>
       <c r="AQ16" t="s">
         <v>16</v>
       </c>
       <c r="AR16">
-        <v>1.83725</v>
+        <v>3.05682</v>
       </c>
       <c r="AS16">
-        <v>2.0531</v>
+        <v>3.2982</v>
       </c>
       <c r="AW16" t="s">
         <v>16</v>
       </c>
       <c r="AX16">
-        <v>2.34927</v>
+        <v>2.07016</v>
       </c>
       <c r="AY16">
-        <v>2.5861</v>
+        <v>2.3055</v>
       </c>
       <c r="BC16" t="s">
         <v>16</v>
       </c>
       <c r="BD16">
-        <v>2.38087</v>
+        <v>4.79841</v>
       </c>
       <c r="BE16">
-        <v>2.557</v>
+        <v>5.0363</v>
       </c>
     </row>
     <row r="17" spans="7:57">
@@ -1658,82 +1658,82 @@
         <v>17</v>
       </c>
       <c r="H17">
-        <v>0.77199</v>
+        <v>0.67025</v>
       </c>
       <c r="I17">
-        <v>1.0196</v>
+        <v>0.911</v>
       </c>
       <c r="M17" t="s">
         <v>17</v>
       </c>
       <c r="N17">
-        <v>0.61064</v>
+        <v>0.69057</v>
       </c>
       <c r="O17">
-        <v>0.8441</v>
+        <v>0.9431</v>
       </c>
       <c r="S17" t="s">
         <v>17</v>
       </c>
       <c r="T17">
-        <v>1.41113</v>
+        <v>1.41506</v>
       </c>
       <c r="U17">
-        <v>1.6334</v>
+        <v>1.666</v>
       </c>
       <c r="Y17" t="s">
         <v>17</v>
       </c>
       <c r="Z17">
-        <v>1.85745</v>
+        <v>2.55691</v>
       </c>
       <c r="AA17">
-        <v>2.0883</v>
+        <v>2.8056</v>
       </c>
       <c r="AE17" t="s">
         <v>17</v>
       </c>
       <c r="AF17">
-        <v>2.41615</v>
+        <v>1.30923</v>
       </c>
       <c r="AG17">
-        <v>2.6341</v>
+        <v>1.5569</v>
       </c>
       <c r="AK17" t="s">
         <v>17</v>
       </c>
       <c r="AL17">
-        <v>1.8019</v>
+        <v>1.42037</v>
       </c>
       <c r="AM17">
-        <v>2.022</v>
+        <v>1.6284</v>
       </c>
       <c r="AQ17" t="s">
         <v>17</v>
       </c>
       <c r="AR17">
-        <v>1.97876</v>
+        <v>2.14078</v>
       </c>
       <c r="AS17">
-        <v>2.1822</v>
+        <v>2.3828</v>
       </c>
       <c r="AW17" t="s">
         <v>17</v>
       </c>
       <c r="AX17">
-        <v>2.15864</v>
+        <v>2.44053</v>
       </c>
       <c r="AY17">
-        <v>2.3971</v>
+        <v>2.6783</v>
       </c>
       <c r="BC17" t="s">
         <v>17</v>
       </c>
       <c r="BD17">
-        <v>3.33956</v>
+        <v>2.83045</v>
       </c>
       <c r="BE17">
-        <v>3.5764</v>
+        <v>3.0126</v>
       </c>
     </row>
     <row r="18" spans="7:57">
@@ -1741,82 +1741,82 @@
         <v>18</v>
       </c>
       <c r="H18">
-        <v>0.9484</v>
+        <v>0.8931</v>
       </c>
       <c r="I18">
-        <v>1.1949</v>
+        <v>1.1332</v>
       </c>
       <c r="M18" t="s">
         <v>18</v>
       </c>
       <c r="N18">
-        <v>1.1098</v>
+        <v>1.5883</v>
       </c>
       <c r="O18">
-        <v>1.3436</v>
+        <v>1.8376</v>
       </c>
       <c r="S18" t="s">
         <v>18</v>
       </c>
       <c r="T18">
-        <v>1.4448</v>
+        <v>1.2663</v>
       </c>
       <c r="U18">
-        <v>1.6795</v>
+        <v>1.5169</v>
       </c>
       <c r="Y18" t="s">
         <v>18</v>
       </c>
       <c r="Z18">
-        <v>2.256</v>
+        <v>2.0716</v>
       </c>
       <c r="AA18">
-        <v>2.4826</v>
+        <v>2.2961</v>
       </c>
       <c r="AE18" t="s">
         <v>18</v>
       </c>
       <c r="AF18">
-        <v>2.114</v>
+        <v>1.7506</v>
       </c>
       <c r="AG18">
-        <v>2.3306</v>
+        <v>1.9975</v>
       </c>
       <c r="AK18" t="s">
         <v>18</v>
       </c>
       <c r="AL18">
-        <v>1.7342</v>
+        <v>1.9738</v>
       </c>
       <c r="AM18">
-        <v>1.9466</v>
+        <v>2.1815</v>
       </c>
       <c r="AQ18" t="s">
         <v>18</v>
       </c>
       <c r="AR18">
-        <v>1.9515</v>
+        <v>2.7849</v>
       </c>
       <c r="AS18">
-        <v>2.1742</v>
+        <v>3.0099</v>
       </c>
       <c r="AW18" t="s">
         <v>18</v>
       </c>
       <c r="AX18">
-        <v>2.1941</v>
+        <v>2.1113</v>
       </c>
       <c r="AY18">
-        <v>2.4156</v>
+        <v>2.3444</v>
       </c>
       <c r="BC18" t="s">
         <v>18</v>
       </c>
       <c r="BD18">
-        <v>2.7795</v>
+        <v>3.1458</v>
       </c>
       <c r="BE18">
-        <v>2.9892</v>
+        <v>3.3776</v>
       </c>
     </row>
     <row r="19" spans="7:57">
@@ -1824,55 +1824,55 @@
         <v>19</v>
       </c>
       <c r="H19">
-        <v>1.8752</v>
+        <v>1.8673</v>
       </c>
       <c r="M19" t="s">
         <v>19</v>
       </c>
       <c r="N19">
-        <v>1.7325</v>
+        <v>1.7528</v>
       </c>
       <c r="S19" t="s">
         <v>19</v>
       </c>
       <c r="T19">
-        <v>1.6349</v>
+        <v>1.6347</v>
       </c>
       <c r="Y19" t="s">
         <v>19</v>
       </c>
       <c r="Z19">
-        <v>1.5587</v>
+        <v>1.5771</v>
       </c>
       <c r="AE19" t="s">
         <v>19</v>
       </c>
       <c r="AF19">
-        <v>1.5862</v>
+        <v>1.5861</v>
       </c>
       <c r="AK19" t="s">
         <v>19</v>
       </c>
       <c r="AL19">
-        <v>1.5515</v>
+        <v>1.5705</v>
       </c>
       <c r="AQ19" t="s">
         <v>19</v>
       </c>
       <c r="AR19">
-        <v>1.5916</v>
+        <v>1.5918</v>
       </c>
       <c r="AW19" t="s">
         <v>19</v>
       </c>
       <c r="AX19">
-        <v>1.5522</v>
+        <v>1.5715</v>
       </c>
       <c r="BC19" t="s">
         <v>19</v>
       </c>
       <c r="BD19">
-        <v>1.5954</v>
+        <v>1.5953</v>
       </c>
     </row>
     <row r="20" spans="7:57">
@@ -1880,13 +1880,13 @@
         <v>20</v>
       </c>
       <c r="H20">
-        <v>0.0086</v>
+        <v>0.008699999999999999</v>
       </c>
       <c r="M20" t="s">
         <v>20</v>
       </c>
       <c r="N20">
-        <v>0.008500000000000001</v>
+        <v>0.008800000000000001</v>
       </c>
       <c r="S20" t="s">
         <v>20</v>
@@ -1904,7 +1904,7 @@
         <v>20</v>
       </c>
       <c r="AF20">
-        <v>0.005</v>
+        <v>0.0049</v>
       </c>
       <c r="AK20" t="s">
         <v>20</v>
@@ -1916,7 +1916,7 @@
         <v>20</v>
       </c>
       <c r="AR20">
-        <v>0.005</v>
+        <v>0.0048</v>
       </c>
       <c r="AW20" t="s">
         <v>20</v>
@@ -1936,7 +1936,7 @@
         <v>21</v>
       </c>
       <c r="H21">
-        <v>0.0878</v>
+        <v>0.0935</v>
       </c>
       <c r="M21" t="s">
         <v>21</v>
@@ -1948,13 +1948,13 @@
         <v>21</v>
       </c>
       <c r="T21">
-        <v>0.07679999999999999</v>
+        <v>0.0769</v>
       </c>
       <c r="Y21" t="s">
         <v>21</v>
       </c>
       <c r="Z21">
-        <v>0.0769</v>
+        <v>0.07729999999999999</v>
       </c>
       <c r="AE21" t="s">
         <v>21</v>
@@ -1966,7 +1966,7 @@
         <v>21</v>
       </c>
       <c r="AL21">
-        <v>0.0766</v>
+        <v>0.0769</v>
       </c>
       <c r="AQ21" t="s">
         <v>21</v>
@@ -1978,7 +1978,7 @@
         <v>21</v>
       </c>
       <c r="AX21">
-        <v>0.0766</v>
+        <v>0.0769</v>
       </c>
       <c r="BC21" t="s">
         <v>21</v>
@@ -1992,37 +1992,37 @@
         <v>22</v>
       </c>
       <c r="H22">
-        <v>1.8838</v>
+        <v>1.876</v>
       </c>
       <c r="M22" t="s">
         <v>22</v>
       </c>
       <c r="N22">
-        <v>1.741</v>
+        <v>1.7616</v>
       </c>
       <c r="S22" t="s">
         <v>22</v>
       </c>
       <c r="T22">
-        <v>1.6406</v>
+        <v>1.6404</v>
       </c>
       <c r="Y22" t="s">
         <v>22</v>
       </c>
       <c r="Z22">
-        <v>1.564</v>
+        <v>1.5824</v>
       </c>
       <c r="AE22" t="s">
         <v>22</v>
       </c>
       <c r="AF22">
-        <v>1.5912</v>
+        <v>1.591</v>
       </c>
       <c r="AK22" t="s">
         <v>22</v>
       </c>
       <c r="AL22">
-        <v>1.5568</v>
+        <v>1.5758</v>
       </c>
       <c r="AQ22" t="s">
         <v>22</v>
@@ -2034,13 +2034,13 @@
         <v>22</v>
       </c>
       <c r="AX22">
-        <v>1.5574</v>
+        <v>1.5767</v>
       </c>
       <c r="BC22" t="s">
         <v>22</v>
       </c>
       <c r="BD22">
-        <v>1.6003</v>
+        <v>1.6002</v>
       </c>
     </row>
     <row r="23" spans="7:57">
@@ -2048,55 +2048,55 @@
         <v>23</v>
       </c>
       <c r="H23">
-        <v>1.963</v>
+        <v>1.9608</v>
       </c>
       <c r="M23" t="s">
         <v>23</v>
       </c>
       <c r="N23">
-        <v>1.8091</v>
+        <v>1.8294</v>
       </c>
       <c r="S23" t="s">
         <v>23</v>
       </c>
       <c r="T23">
-        <v>1.7117</v>
+        <v>1.7116</v>
       </c>
       <c r="Y23" t="s">
         <v>23</v>
       </c>
       <c r="Z23">
-        <v>1.6356</v>
+        <v>1.6544</v>
       </c>
       <c r="AE23" t="s">
         <v>23</v>
       </c>
       <c r="AF23">
-        <v>1.663</v>
+        <v>1.6629</v>
       </c>
       <c r="AK23" t="s">
         <v>23</v>
       </c>
       <c r="AL23">
-        <v>1.6281</v>
+        <v>1.6474</v>
       </c>
       <c r="AQ23" t="s">
         <v>23</v>
       </c>
       <c r="AR23">
-        <v>1.6685</v>
+        <v>1.6687</v>
       </c>
       <c r="AW23" t="s">
         <v>23</v>
       </c>
       <c r="AX23">
-        <v>1.6288</v>
+        <v>1.6484</v>
       </c>
       <c r="BC23" t="s">
         <v>23</v>
       </c>
       <c r="BD23">
-        <v>1.6723</v>
+        <v>1.6722</v>
       </c>
     </row>
     <row r="24" spans="7:57">
@@ -2104,55 +2104,55 @@
         <v>24</v>
       </c>
       <c r="H24">
-        <v>260.07</v>
+        <v>260.932</v>
       </c>
       <c r="M24" t="s">
         <v>24</v>
       </c>
       <c r="N24">
-        <v>264.6266</v>
+        <v>264.5465</v>
       </c>
       <c r="S24" t="s">
         <v>24</v>
       </c>
       <c r="T24">
-        <v>263.9977</v>
+        <v>264.0024</v>
       </c>
       <c r="Y24" t="s">
         <v>24</v>
       </c>
       <c r="Z24">
-        <v>263.7486</v>
+        <v>263.6929</v>
       </c>
       <c r="AE24" t="s">
         <v>24</v>
       </c>
       <c r="AF24">
-        <v>263.5696</v>
+        <v>263.5682</v>
       </c>
       <c r="AK24" t="s">
         <v>24</v>
       </c>
       <c r="AL24">
-        <v>263.7056</v>
+        <v>263.6394</v>
       </c>
       <c r="AQ24" t="s">
         <v>24</v>
       </c>
       <c r="AR24">
-        <v>263.5887</v>
+        <v>263.5877</v>
       </c>
       <c r="AW24" t="s">
         <v>24</v>
       </c>
       <c r="AX24">
-        <v>263.7077</v>
+        <v>263.645</v>
       </c>
       <c r="BC24" t="s">
         <v>24</v>
       </c>
       <c r="BD24">
-        <v>263.5902</v>
+        <v>263.5912</v>
       </c>
     </row>
     <row r="25" spans="7:57">
@@ -2160,55 +2160,55 @@
         <v>25</v>
       </c>
       <c r="H25">
-        <v>260.07</v>
+        <v>260.932</v>
       </c>
       <c r="M25" t="s">
         <v>25</v>
       </c>
       <c r="N25">
-        <v>264.6266</v>
+        <v>264.5465</v>
       </c>
       <c r="S25" t="s">
         <v>25</v>
       </c>
       <c r="T25">
-        <v>263.9977</v>
+        <v>264.0024</v>
       </c>
       <c r="Y25" t="s">
         <v>25</v>
       </c>
       <c r="Z25">
-        <v>263.7486</v>
+        <v>263.6929</v>
       </c>
       <c r="AE25" t="s">
         <v>25</v>
       </c>
       <c r="AF25">
-        <v>263.5696</v>
+        <v>263.5682</v>
       </c>
       <c r="AK25" t="s">
         <v>25</v>
       </c>
       <c r="AL25">
-        <v>263.7056</v>
+        <v>263.6394</v>
       </c>
       <c r="AQ25" t="s">
         <v>25</v>
       </c>
       <c r="AR25">
-        <v>263.5887</v>
+        <v>263.5877</v>
       </c>
       <c r="AW25" t="s">
         <v>25</v>
       </c>
       <c r="AX25">
-        <v>263.7077</v>
+        <v>263.645</v>
       </c>
       <c r="BC25" t="s">
         <v>25</v>
       </c>
       <c r="BD25">
-        <v>263.5902</v>
+        <v>263.5912</v>
       </c>
     </row>
     <row r="26" spans="7:57">
@@ -2216,13 +2216,13 @@
         <v>26</v>
       </c>
       <c r="H26">
-        <v>4.9134</v>
+        <v>4.9059</v>
       </c>
       <c r="M26" t="s">
         <v>26</v>
       </c>
       <c r="N26">
-        <v>4.8779</v>
+        <v>4.8789</v>
       </c>
       <c r="S26" t="s">
         <v>26</v>
@@ -2234,7 +2234,7 @@
         <v>26</v>
       </c>
       <c r="Z26">
-        <v>4.8885</v>
+        <v>4.889</v>
       </c>
       <c r="AE26" t="s">
         <v>26</v>
@@ -2246,7 +2246,7 @@
         <v>26</v>
       </c>
       <c r="AL26">
-        <v>4.8889</v>
+        <v>4.8895</v>
       </c>
       <c r="AQ26" t="s">
         <v>26</v>
@@ -2258,7 +2258,7 @@
         <v>26</v>
       </c>
       <c r="AX26">
-        <v>4.8889</v>
+        <v>4.8895</v>
       </c>
       <c r="BC26" t="s">
         <v>26</v>
@@ -2272,55 +2272,55 @@
         <v>27</v>
       </c>
       <c r="H27">
-        <v>-0.0062</v>
+        <v>-0.0046</v>
       </c>
       <c r="M27" t="s">
         <v>27</v>
       </c>
       <c r="N27">
-        <v>-0.0309</v>
+        <v>-0.0128</v>
       </c>
       <c r="S27" t="s">
         <v>27</v>
       </c>
       <c r="T27">
-        <v>0.0005</v>
+        <v>0.0004</v>
       </c>
       <c r="Y27" t="s">
         <v>27</v>
       </c>
       <c r="Z27">
-        <v>-0.0256</v>
+        <v>-0.0107</v>
       </c>
       <c r="AE27" t="s">
         <v>27</v>
       </c>
       <c r="AF27">
-        <v>0.0083</v>
+        <v>0.008200000000000001</v>
       </c>
       <c r="AK27" t="s">
         <v>27</v>
       </c>
       <c r="AL27">
-        <v>-0.0266</v>
+        <v>-0.0107</v>
       </c>
       <c r="AQ27" t="s">
         <v>27</v>
       </c>
       <c r="AR27">
-        <v>0.012</v>
+        <v>0.0119</v>
       </c>
       <c r="AW27" t="s">
         <v>27</v>
       </c>
       <c r="AX27">
-        <v>-0.0267</v>
+        <v>-0.0107</v>
       </c>
       <c r="BC27" t="s">
         <v>27</v>
       </c>
       <c r="BD27">
-        <v>0.0155</v>
+        <v>0.0154</v>
       </c>
     </row>
     <row r="28" spans="7:57">
@@ -2328,13 +2328,13 @@
         <v>28</v>
       </c>
       <c r="H28">
-        <v>0.7865</v>
+        <v>0.7879</v>
       </c>
       <c r="M28" t="s">
         <v>28</v>
       </c>
       <c r="N28">
-        <v>0.7975</v>
+        <v>0.7978</v>
       </c>
       <c r="S28" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Tracking trajectories in the second level --- Done
</commit_message>
<xml_diff>
--- a/flat_NLP_previous/stats.xlsx
+++ b/flat_NLP_previous/stats.xlsx
@@ -579,82 +579,82 @@
         <v>4</v>
       </c>
       <c r="H4">
-        <v>17.11815</v>
+        <v>12.54361</v>
       </c>
       <c r="I4">
-        <v>17.351</v>
+        <v>12.774</v>
       </c>
       <c r="M4" t="s">
         <v>4</v>
       </c>
       <c r="N4">
-        <v>9.923579999999999</v>
+        <v>34.38618</v>
       </c>
       <c r="O4">
-        <v>10.173</v>
+        <v>34.612</v>
       </c>
       <c r="S4" t="s">
         <v>4</v>
       </c>
       <c r="T4">
-        <v>35.20689</v>
+        <v>24.16274</v>
       </c>
       <c r="U4">
-        <v>35.434</v>
+        <v>24.403</v>
       </c>
       <c r="Y4" t="s">
         <v>4</v>
       </c>
       <c r="Z4">
-        <v>28.71899</v>
+        <v>34.48359</v>
       </c>
       <c r="AA4">
-        <v>28.958</v>
+        <v>34.701</v>
       </c>
       <c r="AE4" t="s">
         <v>4</v>
       </c>
       <c r="AF4">
-        <v>33.56065</v>
+        <v>37.06798</v>
       </c>
       <c r="AG4">
-        <v>33.802</v>
+        <v>37.151</v>
       </c>
       <c r="AK4" t="s">
         <v>4</v>
       </c>
       <c r="AL4">
-        <v>30.53652</v>
+        <v>65.13129000000001</v>
       </c>
       <c r="AM4">
-        <v>30.772</v>
+        <v>65.31</v>
       </c>
       <c r="AQ4" t="s">
         <v>4</v>
       </c>
       <c r="AR4">
-        <v>51.6947</v>
+        <v>56.85228</v>
       </c>
       <c r="AS4">
-        <v>51.928</v>
+        <v>57.075</v>
       </c>
       <c r="AW4" t="s">
         <v>4</v>
       </c>
       <c r="AX4">
-        <v>54.87814</v>
+        <v>67.29371</v>
       </c>
       <c r="AY4">
-        <v>55.108</v>
+        <v>67.512</v>
       </c>
       <c r="BC4" t="s">
         <v>4</v>
       </c>
       <c r="BD4">
-        <v>103.61265</v>
+        <v>83.41866</v>
       </c>
       <c r="BE4">
-        <v>103.83</v>
+        <v>83.621</v>
       </c>
     </row>
     <row r="5" spans="7:57">
@@ -662,82 +662,82 @@
         <v>5</v>
       </c>
       <c r="H5">
-        <v>1.29843</v>
+        <v>2.9384</v>
       </c>
       <c r="I5">
-        <v>1.5392</v>
+        <v>3.1786</v>
       </c>
       <c r="M5" t="s">
         <v>5</v>
       </c>
       <c r="N5">
-        <v>1.42112</v>
+        <v>1.94622</v>
       </c>
       <c r="O5">
-        <v>1.6649</v>
+        <v>2.1681</v>
       </c>
       <c r="S5" t="s">
         <v>5</v>
       </c>
       <c r="T5">
-        <v>7.48784</v>
+        <v>13.54272</v>
       </c>
       <c r="U5">
-        <v>7.7232</v>
+        <v>13.739</v>
       </c>
       <c r="Y5" t="s">
         <v>5</v>
       </c>
       <c r="Z5">
-        <v>22.00877</v>
+        <v>17.21187</v>
       </c>
       <c r="AA5">
-        <v>22.231</v>
+        <v>17.435</v>
       </c>
       <c r="AE5" t="s">
         <v>5</v>
       </c>
       <c r="AF5">
-        <v>21.62376</v>
+        <v>24.64657</v>
       </c>
       <c r="AG5">
-        <v>21.826</v>
+        <v>24.859</v>
       </c>
       <c r="AK5" t="s">
         <v>5</v>
       </c>
       <c r="AL5">
-        <v>12.0057</v>
+        <v>30.43056</v>
       </c>
       <c r="AM5">
-        <v>12.218</v>
+        <v>30.605</v>
       </c>
       <c r="AQ5" t="s">
         <v>5</v>
       </c>
       <c r="AR5">
-        <v>40.43185</v>
+        <v>53.85876</v>
       </c>
       <c r="AS5">
-        <v>40.664</v>
+        <v>54.058</v>
       </c>
       <c r="AW5" t="s">
         <v>5</v>
       </c>
       <c r="AX5">
-        <v>16.93599</v>
+        <v>32.09842</v>
       </c>
       <c r="AY5">
-        <v>17.097</v>
+        <v>32.235</v>
       </c>
       <c r="BC5" t="s">
         <v>5</v>
       </c>
       <c r="BD5">
-        <v>66.14355</v>
+        <v>94.20717999999999</v>
       </c>
       <c r="BE5">
-        <v>66.366</v>
+        <v>94.352</v>
       </c>
     </row>
     <row r="6" spans="7:57">
@@ -745,82 +745,82 @@
         <v>6</v>
       </c>
       <c r="H6">
-        <v>0.42027</v>
+        <v>1.03278</v>
       </c>
       <c r="I6">
-        <v>0.6619</v>
+        <v>1.2422</v>
       </c>
       <c r="M6" t="s">
         <v>6</v>
       </c>
       <c r="N6">
-        <v>0.97806</v>
+        <v>1.56967</v>
       </c>
       <c r="O6">
-        <v>1.2193</v>
+        <v>1.7918</v>
       </c>
       <c r="S6" t="s">
         <v>6</v>
       </c>
       <c r="T6">
-        <v>0.96767</v>
+        <v>2.62161</v>
       </c>
       <c r="U6">
-        <v>1.1895</v>
+        <v>2.8263</v>
       </c>
       <c r="Y6" t="s">
         <v>6</v>
       </c>
       <c r="Z6">
-        <v>3.22111</v>
+        <v>2.30437</v>
       </c>
       <c r="AA6">
-        <v>3.453</v>
+        <v>2.4745</v>
       </c>
       <c r="AE6" t="s">
         <v>6</v>
       </c>
       <c r="AF6">
-        <v>1.9775</v>
+        <v>3.36529</v>
       </c>
       <c r="AG6">
-        <v>2.1805</v>
+        <v>3.5681</v>
       </c>
       <c r="AK6" t="s">
         <v>6</v>
       </c>
       <c r="AL6">
-        <v>2.29607</v>
+        <v>8.44069</v>
       </c>
       <c r="AM6">
-        <v>2.5294</v>
+        <v>8.579599999999999</v>
       </c>
       <c r="AQ6" t="s">
         <v>6</v>
       </c>
       <c r="AR6">
-        <v>3.01492</v>
+        <v>7.01696</v>
       </c>
       <c r="AS6">
-        <v>3.2509</v>
+        <v>7.0945</v>
       </c>
       <c r="AW6" t="s">
         <v>6</v>
       </c>
       <c r="AX6">
-        <v>3.6392</v>
+        <v>6.32687</v>
       </c>
       <c r="AY6">
-        <v>3.8688</v>
+        <v>6.4379</v>
       </c>
       <c r="BC6" t="s">
         <v>6</v>
       </c>
       <c r="BD6">
-        <v>3.30893</v>
+        <v>13.80544</v>
       </c>
       <c r="BE6">
-        <v>3.5385</v>
+        <v>14.002</v>
       </c>
     </row>
     <row r="7" spans="7:57">
@@ -828,82 +828,82 @@
         <v>7</v>
       </c>
       <c r="H7">
-        <v>0.37298</v>
+        <v>0.43689</v>
       </c>
       <c r="I7">
-        <v>0.6241</v>
+        <v>0.6688</v>
       </c>
       <c r="M7" t="s">
         <v>7</v>
       </c>
       <c r="N7">
-        <v>0.64777</v>
+        <v>0.77352</v>
       </c>
       <c r="O7">
-        <v>0.8981</v>
+        <v>1.013</v>
       </c>
       <c r="S7" t="s">
         <v>7</v>
       </c>
       <c r="T7">
-        <v>2.93333</v>
+        <v>1.24489</v>
       </c>
       <c r="U7">
-        <v>3.1509</v>
+        <v>1.4322</v>
       </c>
       <c r="Y7" t="s">
         <v>7</v>
       </c>
       <c r="Z7">
-        <v>1.47886</v>
+        <v>2.1266</v>
       </c>
       <c r="AA7">
-        <v>1.7051</v>
+        <v>2.3314</v>
       </c>
       <c r="AE7" t="s">
         <v>7</v>
       </c>
       <c r="AF7">
-        <v>3.52962</v>
+        <v>7.01153</v>
       </c>
       <c r="AG7">
-        <v>3.7282</v>
+        <v>7.1901</v>
       </c>
       <c r="AK7" t="s">
         <v>7</v>
       </c>
       <c r="AL7">
-        <v>2.06948</v>
+        <v>7.89953</v>
       </c>
       <c r="AM7">
-        <v>2.3102</v>
+        <v>8.074400000000001</v>
       </c>
       <c r="AQ7" t="s">
         <v>7</v>
       </c>
       <c r="AR7">
-        <v>5.86484</v>
+        <v>5.10975</v>
       </c>
       <c r="AS7">
-        <v>6.0878</v>
+        <v>5.2932</v>
       </c>
       <c r="AW7" t="s">
         <v>7</v>
       </c>
       <c r="AX7">
-        <v>3.09327</v>
+        <v>3.24242</v>
       </c>
       <c r="AY7">
-        <v>3.267</v>
+        <v>3.4031</v>
       </c>
       <c r="BC7" t="s">
         <v>7</v>
       </c>
       <c r="BD7">
-        <v>4.16579</v>
+        <v>6.74261</v>
       </c>
       <c r="BE7">
-        <v>4.3232</v>
+        <v>6.8888</v>
       </c>
     </row>
     <row r="8" spans="7:57">
@@ -911,82 +911,82 @@
         <v>8</v>
       </c>
       <c r="H8">
-        <v>0.56863</v>
+        <v>0.45708</v>
       </c>
       <c r="I8">
-        <v>0.8179</v>
+        <v>0.6792</v>
       </c>
       <c r="M8" t="s">
         <v>8</v>
       </c>
       <c r="N8">
-        <v>0.60699</v>
+        <v>0.81786</v>
       </c>
       <c r="O8">
-        <v>0.839</v>
+        <v>1.0411</v>
       </c>
       <c r="S8" t="s">
         <v>8</v>
       </c>
       <c r="T8">
-        <v>0.9458299999999999</v>
+        <v>2.65819</v>
       </c>
       <c r="U8">
-        <v>1.181</v>
+        <v>2.8708</v>
       </c>
       <c r="Y8" t="s">
         <v>8</v>
       </c>
       <c r="Z8">
-        <v>1.59085</v>
+        <v>8.704319999999999</v>
       </c>
       <c r="AA8">
-        <v>1.8247</v>
+        <v>8.9245</v>
       </c>
       <c r="AE8" t="s">
         <v>8</v>
       </c>
       <c r="AF8">
-        <v>1.43501</v>
+        <v>2.49667</v>
       </c>
       <c r="AG8">
-        <v>1.6594</v>
+        <v>2.6747</v>
       </c>
       <c r="AK8" t="s">
         <v>8</v>
       </c>
       <c r="AL8">
-        <v>7.47208</v>
+        <v>4.04099</v>
       </c>
       <c r="AM8">
-        <v>7.6571</v>
+        <v>4.2046</v>
       </c>
       <c r="AQ8" t="s">
         <v>8</v>
       </c>
       <c r="AR8">
-        <v>2.32571</v>
+        <v>4.26978</v>
       </c>
       <c r="AS8">
-        <v>2.5058</v>
+        <v>4.4071</v>
       </c>
       <c r="AW8" t="s">
         <v>8</v>
       </c>
       <c r="AX8">
-        <v>4.15086</v>
+        <v>2.45277</v>
       </c>
       <c r="AY8">
-        <v>4.3243</v>
+        <v>2.6596</v>
       </c>
       <c r="BC8" t="s">
         <v>8</v>
       </c>
       <c r="BD8">
-        <v>2.7789</v>
+        <v>3.68914</v>
       </c>
       <c r="BE8">
-        <v>2.9768</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="9" spans="7:57">
@@ -994,82 +994,82 @@
         <v>9</v>
       </c>
       <c r="H9">
-        <v>0.37499</v>
+        <v>0.59585</v>
       </c>
       <c r="I9">
-        <v>0.6161</v>
+        <v>0.8215</v>
       </c>
       <c r="M9" t="s">
         <v>9</v>
       </c>
       <c r="N9">
-        <v>0.5555600000000001</v>
+        <v>1.0858</v>
       </c>
       <c r="O9">
-        <v>0.784</v>
+        <v>1.3038</v>
       </c>
       <c r="S9" t="s">
         <v>9</v>
       </c>
       <c r="T9">
-        <v>1.1193</v>
+        <v>3.25249</v>
       </c>
       <c r="U9">
-        <v>1.3612</v>
+        <v>3.4333</v>
       </c>
       <c r="Y9" t="s">
         <v>9</v>
       </c>
       <c r="Z9">
-        <v>3.31142</v>
+        <v>3.77853</v>
       </c>
       <c r="AA9">
-        <v>3.5205</v>
+        <v>3.9952</v>
       </c>
       <c r="AE9" t="s">
         <v>9</v>
       </c>
       <c r="AF9">
-        <v>5.36774</v>
+        <v>2.69743</v>
       </c>
       <c r="AG9">
-        <v>5.5666</v>
+        <v>2.9043</v>
       </c>
       <c r="AK9" t="s">
         <v>9</v>
       </c>
       <c r="AL9">
-        <v>1.8903</v>
+        <v>2.52132</v>
       </c>
       <c r="AM9">
-        <v>2.0754</v>
+        <v>2.7142</v>
       </c>
       <c r="AQ9" t="s">
         <v>9</v>
       </c>
       <c r="AR9">
-        <v>2.80809</v>
+        <v>2.81318</v>
       </c>
       <c r="AS9">
-        <v>3.0425</v>
+        <v>2.9994</v>
       </c>
       <c r="AW9" t="s">
         <v>9</v>
       </c>
       <c r="AX9">
-        <v>3.11954</v>
+        <v>4.10984</v>
       </c>
       <c r="AY9">
-        <v>3.3286</v>
+        <v>4.3109</v>
       </c>
       <c r="BC9" t="s">
         <v>9</v>
       </c>
       <c r="BD9">
-        <v>3.3353</v>
+        <v>20.53137</v>
       </c>
       <c r="BE9">
-        <v>3.4907</v>
+        <v>20.663</v>
       </c>
     </row>
     <row r="10" spans="7:57">
@@ -1077,82 +1077,82 @@
         <v>10</v>
       </c>
       <c r="H10">
-        <v>0.29399</v>
+        <v>0.54453</v>
       </c>
       <c r="I10">
-        <v>0.5492</v>
+        <v>0.7803</v>
       </c>
       <c r="M10" t="s">
         <v>10</v>
       </c>
       <c r="N10">
-        <v>0.82611</v>
+        <v>0.9057500000000001</v>
       </c>
       <c r="O10">
-        <v>1.0725</v>
+        <v>1.1128</v>
       </c>
       <c r="S10" t="s">
         <v>10</v>
       </c>
       <c r="T10">
-        <v>1.90118</v>
+        <v>0.8969200000000001</v>
       </c>
       <c r="U10">
-        <v>2.139</v>
+        <v>1.1037</v>
       </c>
       <c r="Y10" t="s">
         <v>10</v>
       </c>
       <c r="Z10">
-        <v>1.78053</v>
+        <v>7.27252</v>
       </c>
       <c r="AA10">
-        <v>2.0091</v>
+        <v>7.46</v>
       </c>
       <c r="AE10" t="s">
         <v>10</v>
       </c>
       <c r="AF10">
-        <v>1.52806</v>
+        <v>8.792260000000001</v>
       </c>
       <c r="AG10">
-        <v>1.7665</v>
+        <v>8.9765</v>
       </c>
       <c r="AK10" t="s">
         <v>10</v>
       </c>
       <c r="AL10">
-        <v>3.35794</v>
+        <v>2.39982</v>
       </c>
       <c r="AM10">
-        <v>3.5506</v>
+        <v>2.6048</v>
       </c>
       <c r="AQ10" t="s">
         <v>10</v>
       </c>
       <c r="AR10">
-        <v>2.3828</v>
+        <v>7.44882</v>
       </c>
       <c r="AS10">
-        <v>2.5625</v>
+        <v>7.647</v>
       </c>
       <c r="AW10" t="s">
         <v>10</v>
       </c>
       <c r="AX10">
-        <v>9.336690000000001</v>
+        <v>3.57733</v>
       </c>
       <c r="AY10">
-        <v>9.568</v>
+        <v>3.7988</v>
       </c>
       <c r="BC10" t="s">
         <v>10</v>
       </c>
       <c r="BD10">
-        <v>3.15687</v>
+        <v>4.02658</v>
       </c>
       <c r="BE10">
-        <v>3.3851</v>
+        <v>4.2195</v>
       </c>
     </row>
     <row r="11" spans="7:57">
@@ -1160,82 +1160,82 @@
         <v>11</v>
       </c>
       <c r="H11">
-        <v>0.33039</v>
+        <v>0.51486</v>
       </c>
       <c r="I11">
-        <v>0.5793</v>
+        <v>0.727</v>
       </c>
       <c r="M11" t="s">
         <v>11</v>
       </c>
       <c r="N11">
-        <v>0.61966</v>
+        <v>1.30555</v>
       </c>
       <c r="O11">
-        <v>0.867</v>
+        <v>1.5114</v>
       </c>
       <c r="S11" t="s">
         <v>11</v>
       </c>
       <c r="T11">
-        <v>3.51705</v>
+        <v>1.49013</v>
       </c>
       <c r="U11">
-        <v>3.7592</v>
+        <v>1.7082</v>
       </c>
       <c r="Y11" t="s">
         <v>11</v>
       </c>
       <c r="Z11">
-        <v>3.28297</v>
+        <v>1.67424</v>
       </c>
       <c r="AA11">
-        <v>3.5087</v>
+        <v>1.8645</v>
       </c>
       <c r="AE11" t="s">
         <v>11</v>
       </c>
       <c r="AF11">
-        <v>1.94119</v>
+        <v>3.5213</v>
       </c>
       <c r="AG11">
-        <v>2.1648</v>
+        <v>3.7129</v>
       </c>
       <c r="AK11" t="s">
         <v>11</v>
       </c>
       <c r="AL11">
-        <v>2.35183</v>
+        <v>2.78334</v>
       </c>
       <c r="AM11">
-        <v>2.5447</v>
+        <v>2.9773</v>
       </c>
       <c r="AQ11" t="s">
         <v>11</v>
       </c>
       <c r="AR11">
-        <v>2.71369</v>
+        <v>3.02422</v>
       </c>
       <c r="AS11">
-        <v>2.8869</v>
+        <v>3.1809</v>
       </c>
       <c r="AW11" t="s">
         <v>11</v>
       </c>
       <c r="AX11">
-        <v>3.33541</v>
+        <v>3.60067</v>
       </c>
       <c r="AY11">
-        <v>3.5654</v>
+        <v>3.7401</v>
       </c>
       <c r="BC11" t="s">
         <v>11</v>
       </c>
       <c r="BD11">
-        <v>4.1785</v>
+        <v>3.50832</v>
       </c>
       <c r="BE11">
-        <v>4.3466</v>
+        <v>3.6751</v>
       </c>
     </row>
     <row r="12" spans="7:57">
@@ -1243,82 +1243,82 @@
         <v>12</v>
       </c>
       <c r="H12">
-        <v>0.27383</v>
+        <v>0.43876</v>
       </c>
       <c r="I12">
-        <v>0.5261</v>
+        <v>0.6666</v>
       </c>
       <c r="M12" t="s">
         <v>12</v>
       </c>
       <c r="N12">
-        <v>1.01317</v>
+        <v>2.10773</v>
       </c>
       <c r="O12">
-        <v>1.2622</v>
+        <v>2.3435</v>
       </c>
       <c r="S12" t="s">
         <v>12</v>
       </c>
       <c r="T12">
-        <v>2.6642</v>
+        <v>4.1506</v>
       </c>
       <c r="U12">
-        <v>2.8858</v>
+        <v>4.3107</v>
       </c>
       <c r="Y12" t="s">
         <v>12</v>
       </c>
       <c r="Z12">
-        <v>1.69141</v>
+        <v>8.158620000000001</v>
       </c>
       <c r="AA12">
-        <v>1.9035</v>
+        <v>8.3515</v>
       </c>
       <c r="AE12" t="s">
         <v>12</v>
       </c>
       <c r="AF12">
-        <v>2.09308</v>
+        <v>4.12562</v>
       </c>
       <c r="AG12">
-        <v>2.2995</v>
+        <v>4.3021</v>
       </c>
       <c r="AK12" t="s">
         <v>12</v>
       </c>
       <c r="AL12">
-        <v>2.58784</v>
+        <v>2.50076</v>
       </c>
       <c r="AM12">
-        <v>2.8225</v>
+        <v>2.6892</v>
       </c>
       <c r="AQ12" t="s">
         <v>12</v>
       </c>
       <c r="AR12">
-        <v>2.59346</v>
+        <v>5.82736</v>
       </c>
       <c r="AS12">
-        <v>2.7745</v>
+        <v>6.0305</v>
       </c>
       <c r="AW12" t="s">
         <v>12</v>
       </c>
       <c r="AX12">
-        <v>2.97293</v>
+        <v>2.98443</v>
       </c>
       <c r="AY12">
-        <v>3.2051</v>
+        <v>3.1755</v>
       </c>
       <c r="BC12" t="s">
         <v>12</v>
       </c>
       <c r="BD12">
-        <v>8.775090000000001</v>
+        <v>4.14827</v>
       </c>
       <c r="BE12">
-        <v>9.0069</v>
+        <v>4.2951</v>
       </c>
     </row>
     <row r="13" spans="7:57">
@@ -1326,82 +1326,82 @@
         <v>13</v>
       </c>
       <c r="H13">
-        <v>0.31429</v>
+        <v>0.74736</v>
       </c>
       <c r="I13">
-        <v>0.5691000000000001</v>
+        <v>0.9841</v>
       </c>
       <c r="M13" t="s">
         <v>13</v>
       </c>
       <c r="N13">
-        <v>0.67501</v>
+        <v>1.44472</v>
       </c>
       <c r="O13">
-        <v>0.9149</v>
+        <v>1.6584</v>
       </c>
       <c r="S13" t="s">
         <v>13</v>
       </c>
       <c r="T13">
-        <v>1.17807</v>
+        <v>10.28082</v>
       </c>
       <c r="U13">
-        <v>1.4244</v>
+        <v>10.47</v>
       </c>
       <c r="Y13" t="s">
         <v>13</v>
       </c>
       <c r="Z13">
-        <v>1.56508</v>
+        <v>1.51325</v>
       </c>
       <c r="AA13">
-        <v>1.7709</v>
+        <v>1.7126</v>
       </c>
       <c r="AE13" t="s">
         <v>13</v>
       </c>
       <c r="AF13">
-        <v>2.09885</v>
+        <v>10.45175</v>
       </c>
       <c r="AG13">
-        <v>2.2731</v>
+        <v>10.639</v>
       </c>
       <c r="AK13" t="s">
         <v>13</v>
       </c>
       <c r="AL13">
-        <v>2.26057</v>
+        <v>2.93385</v>
       </c>
       <c r="AM13">
-        <v>2.478</v>
+        <v>3.1178</v>
       </c>
       <c r="AQ13" t="s">
         <v>13</v>
       </c>
       <c r="AR13">
-        <v>7.15043</v>
+        <v>2.92548</v>
       </c>
       <c r="AS13">
-        <v>7.3612</v>
+        <v>3.1329</v>
       </c>
       <c r="AW13" t="s">
         <v>13</v>
       </c>
       <c r="AX13">
-        <v>5.14278</v>
+        <v>3.74994</v>
       </c>
       <c r="AY13">
-        <v>5.3716</v>
+        <v>3.8879</v>
       </c>
       <c r="BC13" t="s">
         <v>13</v>
       </c>
       <c r="BD13">
-        <v>4.28052</v>
+        <v>4.03775</v>
       </c>
       <c r="BE13">
-        <v>4.5099</v>
+        <v>4.1384</v>
       </c>
     </row>
     <row r="14" spans="7:57">
@@ -1409,82 +1409,82 @@
         <v>14</v>
       </c>
       <c r="H14">
-        <v>0.38583</v>
+        <v>0.4448</v>
       </c>
       <c r="I14">
-        <v>0.6319</v>
+        <v>0.6757</v>
       </c>
       <c r="M14" t="s">
         <v>14</v>
       </c>
       <c r="N14">
-        <v>0.66604</v>
+        <v>0.96855</v>
       </c>
       <c r="O14">
-        <v>0.9104</v>
+        <v>1.1589</v>
       </c>
       <c r="S14" t="s">
         <v>14</v>
       </c>
       <c r="T14">
-        <v>1.25052</v>
+        <v>1.02987</v>
       </c>
       <c r="U14">
-        <v>1.4866</v>
+        <v>1.2587</v>
       </c>
       <c r="Y14" t="s">
         <v>14</v>
       </c>
       <c r="Z14">
-        <v>2.0046</v>
+        <v>5.55761</v>
       </c>
       <c r="AA14">
-        <v>2.2369</v>
+        <v>5.7019</v>
       </c>
       <c r="AE14" t="s">
         <v>14</v>
       </c>
       <c r="AF14">
-        <v>1.64334</v>
+        <v>2.32135</v>
       </c>
       <c r="AG14">
-        <v>1.885</v>
+        <v>2.5256</v>
       </c>
       <c r="AK14" t="s">
         <v>14</v>
       </c>
       <c r="AL14">
-        <v>2.2894</v>
+        <v>3.24687</v>
       </c>
       <c r="AM14">
-        <v>2.4814</v>
+        <v>3.434</v>
       </c>
       <c r="AQ14" t="s">
         <v>14</v>
       </c>
       <c r="AR14">
-        <v>2.6477</v>
+        <v>3.08916</v>
       </c>
       <c r="AS14">
-        <v>2.8324</v>
+        <v>3.2449</v>
       </c>
       <c r="AW14" t="s">
         <v>14</v>
       </c>
       <c r="AX14">
-        <v>6.09834</v>
+        <v>3.37187</v>
       </c>
       <c r="AY14">
-        <v>6.3031</v>
+        <v>3.5868</v>
       </c>
       <c r="BC14" t="s">
         <v>14</v>
       </c>
       <c r="BD14">
-        <v>5.08395</v>
+        <v>6.22291</v>
       </c>
       <c r="BE14">
-        <v>5.3148</v>
+        <v>6.3688</v>
       </c>
     </row>
     <row r="15" spans="7:57">
@@ -1492,82 +1492,82 @@
         <v>15</v>
       </c>
       <c r="H15">
-        <v>0.3401</v>
+        <v>0.45231</v>
       </c>
       <c r="I15">
-        <v>0.5802</v>
+        <v>0.6901</v>
       </c>
       <c r="M15" t="s">
         <v>15</v>
       </c>
       <c r="N15">
-        <v>0.73246</v>
+        <v>2.00398</v>
       </c>
       <c r="O15">
-        <v>0.9822</v>
+        <v>2.2287</v>
       </c>
       <c r="S15" t="s">
         <v>15</v>
       </c>
       <c r="T15">
-        <v>1.04981</v>
+        <v>5.59461</v>
       </c>
       <c r="U15">
-        <v>1.2824</v>
+        <v>5.7283</v>
       </c>
       <c r="Y15" t="s">
         <v>15</v>
       </c>
       <c r="Z15">
-        <v>3.62995</v>
+        <v>1.84623</v>
       </c>
       <c r="AA15">
-        <v>3.8592</v>
+        <v>2.0547</v>
       </c>
       <c r="AE15" t="s">
         <v>15</v>
       </c>
       <c r="AF15">
-        <v>2.03901</v>
+        <v>2.13765</v>
       </c>
       <c r="AG15">
-        <v>2.2788</v>
+        <v>2.2629</v>
       </c>
       <c r="AK15" t="s">
         <v>15</v>
       </c>
       <c r="AL15">
-        <v>1.86788</v>
+        <v>2.77704</v>
       </c>
       <c r="AM15">
-        <v>2.0577</v>
+        <v>2.9665</v>
       </c>
       <c r="AQ15" t="s">
         <v>15</v>
       </c>
       <c r="AR15">
-        <v>2.66681</v>
+        <v>2.69353</v>
       </c>
       <c r="AS15">
-        <v>2.8776</v>
+        <v>2.8624</v>
       </c>
       <c r="AW15" t="s">
         <v>15</v>
       </c>
       <c r="AX15">
-        <v>2.23344</v>
+        <v>3.32739</v>
       </c>
       <c r="AY15">
-        <v>2.4024</v>
+        <v>3.4699</v>
       </c>
       <c r="BC15" t="s">
         <v>15</v>
       </c>
       <c r="BD15">
-        <v>4.09636</v>
+        <v>4.20136</v>
       </c>
       <c r="BE15">
-        <v>4.3243</v>
+        <v>4.3195</v>
       </c>
     </row>
     <row r="16" spans="7:57">
@@ -1575,82 +1575,82 @@
         <v>16</v>
       </c>
       <c r="H16">
-        <v>0.43827</v>
+        <v>0.41458</v>
       </c>
       <c r="I16">
-        <v>0.6781</v>
+        <v>0.642</v>
       </c>
       <c r="M16" t="s">
         <v>16</v>
       </c>
       <c r="N16">
-        <v>0.70844</v>
+        <v>2.67889</v>
       </c>
       <c r="O16">
-        <v>0.9415</v>
+        <v>2.9074</v>
       </c>
       <c r="S16" t="s">
         <v>16</v>
       </c>
       <c r="T16">
-        <v>1.0234</v>
+        <v>2.67488</v>
       </c>
       <c r="U16">
-        <v>1.2423</v>
+        <v>2.876</v>
       </c>
       <c r="Y16" t="s">
         <v>16</v>
       </c>
       <c r="Z16">
-        <v>1.63389</v>
+        <v>5.6341</v>
       </c>
       <c r="AA16">
-        <v>1.8664</v>
+        <v>5.8218</v>
       </c>
       <c r="AE16" t="s">
         <v>16</v>
       </c>
       <c r="AF16">
-        <v>1.82536</v>
+        <v>4.65102</v>
       </c>
       <c r="AG16">
-        <v>2.0499</v>
+        <v>4.8735</v>
       </c>
       <c r="AK16" t="s">
         <v>16</v>
       </c>
       <c r="AL16">
-        <v>2.10898</v>
+        <v>3.60013</v>
       </c>
       <c r="AM16">
-        <v>2.3475</v>
+        <v>3.78</v>
       </c>
       <c r="AQ16" t="s">
         <v>16</v>
       </c>
       <c r="AR16">
-        <v>2.68555</v>
+        <v>3.23274</v>
       </c>
       <c r="AS16">
-        <v>2.864</v>
+        <v>3.4042</v>
       </c>
       <c r="AW16" t="s">
         <v>16</v>
       </c>
       <c r="AX16">
-        <v>3.39632</v>
+        <v>3.65347</v>
       </c>
       <c r="AY16">
-        <v>3.6239</v>
+        <v>3.7583</v>
       </c>
       <c r="BC16" t="s">
         <v>16</v>
       </c>
       <c r="BD16">
-        <v>4.65725</v>
+        <v>4.05932</v>
       </c>
       <c r="BE16">
-        <v>4.8225</v>
+        <v>4.1546</v>
       </c>
     </row>
     <row r="17" spans="7:57">
@@ -1658,82 +1658,82 @@
         <v>17</v>
       </c>
       <c r="H17">
-        <v>0.34209</v>
+        <v>0.42274</v>
       </c>
       <c r="I17">
-        <v>0.5903</v>
+        <v>0.6552</v>
       </c>
       <c r="M17" t="s">
         <v>17</v>
       </c>
       <c r="N17">
-        <v>0.66753</v>
+        <v>3.01786</v>
       </c>
       <c r="O17">
-        <v>0.9049</v>
+        <v>3.2159</v>
       </c>
       <c r="S17" t="s">
         <v>17</v>
       </c>
       <c r="T17">
-        <v>14.04684</v>
+        <v>1.41064</v>
       </c>
       <c r="U17">
-        <v>14.289</v>
+        <v>1.6462</v>
       </c>
       <c r="Y17" t="s">
         <v>17</v>
       </c>
       <c r="Z17">
-        <v>1.77525</v>
+        <v>4.96597</v>
       </c>
       <c r="AA17">
-        <v>2.0131</v>
+        <v>5.1625</v>
       </c>
       <c r="AE17" t="s">
         <v>17</v>
       </c>
       <c r="AF17">
-        <v>2.01974</v>
+        <v>2.96044</v>
       </c>
       <c r="AG17">
-        <v>2.2242</v>
+        <v>3.1712</v>
       </c>
       <c r="AK17" t="s">
         <v>17</v>
       </c>
       <c r="AL17">
-        <v>2.49307</v>
+        <v>3.29684</v>
       </c>
       <c r="AM17">
-        <v>2.7329</v>
+        <v>3.508</v>
       </c>
       <c r="AQ17" t="s">
         <v>17</v>
       </c>
       <c r="AR17">
-        <v>2.85116</v>
+        <v>3.14982</v>
       </c>
       <c r="AS17">
-        <v>3.0874</v>
+        <v>3.3539</v>
       </c>
       <c r="AW17" t="s">
         <v>17</v>
       </c>
       <c r="AX17">
-        <v>3.25755</v>
+        <v>3.29725</v>
       </c>
       <c r="AY17">
-        <v>3.4286</v>
+        <v>3.4451</v>
       </c>
       <c r="BC17" t="s">
         <v>17</v>
       </c>
       <c r="BD17">
-        <v>3.55713</v>
+        <v>3.58336</v>
       </c>
       <c r="BE17">
-        <v>3.7865</v>
+        <v>3.7442</v>
       </c>
     </row>
     <row r="18" spans="7:57">
@@ -1741,82 +1741,82 @@
         <v>18</v>
       </c>
       <c r="H18">
-        <v>0.3713</v>
+        <v>0.5419</v>
       </c>
       <c r="I18">
-        <v>0.6187</v>
+        <v>0.7694</v>
       </c>
       <c r="M18" t="s">
         <v>18</v>
       </c>
       <c r="N18">
-        <v>0.7247</v>
+        <v>1.5567</v>
       </c>
       <c r="O18">
-        <v>0.9663</v>
+        <v>1.7739</v>
       </c>
       <c r="S18" t="s">
         <v>18</v>
       </c>
       <c r="T18">
-        <v>2.7164</v>
+        <v>3.1088</v>
       </c>
       <c r="U18">
-        <v>2.9493</v>
+        <v>3.3054</v>
       </c>
       <c r="Y18" t="s">
         <v>18</v>
       </c>
       <c r="Z18">
-        <v>2.2472</v>
+        <v>4.4614</v>
       </c>
       <c r="AA18">
-        <v>2.4726</v>
+        <v>4.6546</v>
       </c>
       <c r="AE18" t="s">
         <v>18</v>
       </c>
       <c r="AF18">
-        <v>2.2915</v>
+        <v>4.5444</v>
       </c>
       <c r="AG18">
-        <v>2.5064</v>
+        <v>4.7334</v>
       </c>
       <c r="AK18" t="s">
         <v>18</v>
       </c>
       <c r="AL18">
-        <v>2.7538</v>
+        <v>3.8701</v>
       </c>
       <c r="AM18">
-        <v>2.9656</v>
+        <v>4.0542</v>
       </c>
       <c r="AQ18" t="s">
         <v>18</v>
       </c>
       <c r="AR18">
-        <v>3.3088</v>
+        <v>4.2167</v>
       </c>
       <c r="AS18">
-        <v>3.5111</v>
+        <v>4.3876</v>
       </c>
       <c r="AW18" t="s">
         <v>18</v>
       </c>
       <c r="AX18">
-        <v>4.148</v>
+        <v>3.6412</v>
       </c>
       <c r="AY18">
-        <v>4.3547</v>
+        <v>3.8062</v>
       </c>
       <c r="BC18" t="s">
         <v>18</v>
       </c>
       <c r="BD18">
-        <v>4.2812</v>
+        <v>6.5464</v>
       </c>
       <c r="BE18">
-        <v>4.4855</v>
+        <v>6.6958</v>
       </c>
     </row>
     <row r="19" spans="7:57">
@@ -1824,55 +1824,55 @@
         <v>19</v>
       </c>
       <c r="H19">
-        <v>4.34</v>
+        <v>5.1413</v>
       </c>
       <c r="M19" t="s">
         <v>19</v>
       </c>
       <c r="N19">
-        <v>2.7281</v>
+        <v>3.7761</v>
       </c>
       <c r="S19" t="s">
         <v>19</v>
       </c>
       <c r="T19">
-        <v>1.8051</v>
+        <v>2.6348</v>
       </c>
       <c r="Y19" t="s">
         <v>19</v>
       </c>
       <c r="Z19">
-        <v>1.4484</v>
+        <v>2.2479</v>
       </c>
       <c r="AE19" t="s">
         <v>19</v>
       </c>
       <c r="AF19">
-        <v>1.4563</v>
+        <v>2.2198</v>
       </c>
       <c r="AK19" t="s">
         <v>19</v>
       </c>
       <c r="AL19">
-        <v>1.4262</v>
+        <v>2.2189</v>
       </c>
       <c r="AQ19" t="s">
         <v>19</v>
       </c>
       <c r="AR19">
-        <v>1.452</v>
+        <v>2.2203</v>
       </c>
       <c r="AW19" t="s">
         <v>19</v>
       </c>
       <c r="AX19">
-        <v>1.4463</v>
+        <v>2.2204</v>
       </c>
       <c r="BC19" t="s">
         <v>19</v>
       </c>
       <c r="BD19">
-        <v>1.4533</v>
+        <v>2.2204</v>
       </c>
     </row>
     <row r="20" spans="7:57">
@@ -1880,55 +1880,55 @@
         <v>20</v>
       </c>
       <c r="H20">
-        <v>0.2686</v>
+        <v>0.0888</v>
       </c>
       <c r="M20" t="s">
         <v>20</v>
       </c>
       <c r="N20">
-        <v>0.3906</v>
+        <v>0.5059</v>
       </c>
       <c r="S20" t="s">
         <v>20</v>
       </c>
       <c r="T20">
-        <v>0.0252</v>
+        <v>0.0173</v>
       </c>
       <c r="Y20" t="s">
         <v>20</v>
       </c>
       <c r="Z20">
-        <v>0.0107</v>
+        <v>0.0121</v>
       </c>
       <c r="AE20" t="s">
         <v>20</v>
       </c>
       <c r="AF20">
-        <v>0.009599999999999999</v>
+        <v>0.0107</v>
       </c>
       <c r="AK20" t="s">
         <v>20</v>
       </c>
       <c r="AL20">
-        <v>0.0097</v>
+        <v>0.0107</v>
       </c>
       <c r="AQ20" t="s">
         <v>20</v>
       </c>
       <c r="AR20">
-        <v>0.0091</v>
+        <v>0.0108</v>
       </c>
       <c r="AW20" t="s">
         <v>20</v>
       </c>
       <c r="AX20">
-        <v>0.0097</v>
+        <v>0.0108</v>
       </c>
       <c r="BC20" t="s">
         <v>20</v>
       </c>
       <c r="BD20">
-        <v>0.0089</v>
+        <v>0.0108</v>
       </c>
     </row>
     <row r="21" spans="7:57">
@@ -1936,55 +1936,55 @@
         <v>21</v>
       </c>
       <c r="H21">
-        <v>0.1859</v>
+        <v>0.1749</v>
       </c>
       <c r="M21" t="s">
         <v>21</v>
       </c>
       <c r="N21">
-        <v>0.0711</v>
+        <v>0.1027</v>
       </c>
       <c r="S21" t="s">
         <v>21</v>
       </c>
       <c r="T21">
-        <v>0.0377</v>
+        <v>0.0571</v>
       </c>
       <c r="Y21" t="s">
         <v>21</v>
       </c>
       <c r="Z21">
-        <v>0.037</v>
+        <v>0.0526</v>
       </c>
       <c r="AE21" t="s">
         <v>21</v>
       </c>
       <c r="AF21">
-        <v>0.0361</v>
+        <v>0.0518</v>
       </c>
       <c r="AK21" t="s">
         <v>21</v>
       </c>
       <c r="AL21">
-        <v>0.0364</v>
+        <v>0.0518</v>
       </c>
       <c r="AQ21" t="s">
         <v>21</v>
       </c>
       <c r="AR21">
-        <v>0.036</v>
+        <v>0.0518</v>
       </c>
       <c r="AW21" t="s">
         <v>21</v>
       </c>
       <c r="AX21">
-        <v>0.0365</v>
+        <v>0.0518</v>
       </c>
       <c r="BC21" t="s">
         <v>21</v>
       </c>
       <c r="BD21">
-        <v>0.036</v>
+        <v>0.0518</v>
       </c>
     </row>
     <row r="22" spans="7:57">
@@ -1992,55 +1992,55 @@
         <v>22</v>
       </c>
       <c r="H22">
-        <v>4.6086</v>
+        <v>5.2301</v>
       </c>
       <c r="M22" t="s">
         <v>22</v>
       </c>
       <c r="N22">
-        <v>3.1187</v>
+        <v>4.282</v>
       </c>
       <c r="S22" t="s">
         <v>22</v>
       </c>
       <c r="T22">
-        <v>1.8303</v>
+        <v>2.6521</v>
       </c>
       <c r="Y22" t="s">
         <v>22</v>
       </c>
       <c r="Z22">
-        <v>1.4591</v>
+        <v>2.26</v>
       </c>
       <c r="AE22" t="s">
         <v>22</v>
       </c>
       <c r="AF22">
-        <v>1.4659</v>
+        <v>2.2305</v>
       </c>
       <c r="AK22" t="s">
         <v>22</v>
       </c>
       <c r="AL22">
-        <v>1.4359</v>
+        <v>2.2296</v>
       </c>
       <c r="AQ22" t="s">
         <v>22</v>
       </c>
       <c r="AR22">
-        <v>1.4611</v>
+        <v>2.2311</v>
       </c>
       <c r="AW22" t="s">
         <v>22</v>
       </c>
       <c r="AX22">
-        <v>1.456</v>
+        <v>2.2312</v>
       </c>
       <c r="BC22" t="s">
         <v>22</v>
       </c>
       <c r="BD22">
-        <v>1.4622</v>
+        <v>2.2312</v>
       </c>
     </row>
     <row r="23" spans="7:57">
@@ -2048,55 +2048,55 @@
         <v>23</v>
       </c>
       <c r="H23">
-        <v>4.5259</v>
+        <v>5.3162</v>
       </c>
       <c r="M23" t="s">
         <v>23</v>
       </c>
       <c r="N23">
-        <v>2.7992</v>
+        <v>3.8788</v>
       </c>
       <c r="S23" t="s">
         <v>23</v>
       </c>
       <c r="T23">
-        <v>1.8428</v>
+        <v>2.6919</v>
       </c>
       <c r="Y23" t="s">
         <v>23</v>
       </c>
       <c r="Z23">
-        <v>1.4854</v>
+        <v>2.3005</v>
       </c>
       <c r="AE23" t="s">
         <v>23</v>
       </c>
       <c r="AF23">
-        <v>1.4924</v>
+        <v>2.2716</v>
       </c>
       <c r="AK23" t="s">
         <v>23</v>
       </c>
       <c r="AL23">
-        <v>1.4626</v>
+        <v>2.2707</v>
       </c>
       <c r="AQ23" t="s">
         <v>23</v>
       </c>
       <c r="AR23">
-        <v>1.488</v>
+        <v>2.2721</v>
       </c>
       <c r="AW23" t="s">
         <v>23</v>
       </c>
       <c r="AX23">
-        <v>1.4828</v>
+        <v>2.2722</v>
       </c>
       <c r="BC23" t="s">
         <v>23</v>
       </c>
       <c r="BD23">
-        <v>1.4893</v>
+        <v>2.2722</v>
       </c>
     </row>
     <row r="24" spans="7:57">
@@ -2104,55 +2104,55 @@
         <v>24</v>
       </c>
       <c r="H24">
-        <v>251.9507</v>
+        <v>2223.5675</v>
       </c>
       <c r="M24" t="s">
         <v>24</v>
       </c>
       <c r="N24">
-        <v>266.1234</v>
+        <v>2267.2191</v>
       </c>
       <c r="S24" t="s">
         <v>24</v>
       </c>
       <c r="T24">
-        <v>260.6586</v>
+        <v>2250.321</v>
       </c>
       <c r="Y24" t="s">
         <v>24</v>
       </c>
       <c r="Z24">
-        <v>261.2448</v>
+        <v>2248.763</v>
       </c>
       <c r="AE24" t="s">
         <v>24</v>
       </c>
       <c r="AF24">
-        <v>260.9916</v>
+        <v>2247.9276</v>
       </c>
       <c r="AK24" t="s">
         <v>24</v>
       </c>
       <c r="AL24">
-        <v>261.0163</v>
+        <v>2247.9327</v>
       </c>
       <c r="AQ24" t="s">
         <v>24</v>
       </c>
       <c r="AR24">
-        <v>260.9542</v>
+        <v>2247.9733</v>
       </c>
       <c r="AW24" t="s">
         <v>24</v>
       </c>
       <c r="AX24">
-        <v>260.8946</v>
+        <v>2247.9753</v>
       </c>
       <c r="BC24" t="s">
         <v>24</v>
       </c>
       <c r="BD24">
-        <v>260.9551</v>
+        <v>2247.9638</v>
       </c>
     </row>
     <row r="25" spans="7:57">
@@ -2160,55 +2160,55 @@
         <v>25</v>
       </c>
       <c r="H25">
-        <v>251.9507</v>
+        <v>2223.5675</v>
       </c>
       <c r="M25" t="s">
         <v>25</v>
       </c>
       <c r="N25">
-        <v>266.1234</v>
+        <v>2267.2191</v>
       </c>
       <c r="S25" t="s">
         <v>25</v>
       </c>
       <c r="T25">
-        <v>260.6586</v>
+        <v>2250.321</v>
       </c>
       <c r="Y25" t="s">
         <v>25</v>
       </c>
       <c r="Z25">
-        <v>261.2448</v>
+        <v>2248.763</v>
       </c>
       <c r="AE25" t="s">
         <v>25</v>
       </c>
       <c r="AF25">
-        <v>260.9916</v>
+        <v>2247.9276</v>
       </c>
       <c r="AK25" t="s">
         <v>25</v>
       </c>
       <c r="AL25">
-        <v>261.0163</v>
+        <v>2247.9327</v>
       </c>
       <c r="AQ25" t="s">
         <v>25</v>
       </c>
       <c r="AR25">
-        <v>260.9542</v>
+        <v>2247.9733</v>
       </c>
       <c r="AW25" t="s">
         <v>25</v>
       </c>
       <c r="AX25">
-        <v>260.8946</v>
+        <v>2247.9753</v>
       </c>
       <c r="BC25" t="s">
         <v>25</v>
       </c>
       <c r="BD25">
-        <v>260.9551</v>
+        <v>2247.9638</v>
       </c>
     </row>
     <row r="26" spans="7:57">
@@ -2216,55 +2216,55 @@
         <v>26</v>
       </c>
       <c r="H26">
-        <v>4.9979</v>
+        <v>5.0957</v>
       </c>
       <c r="M26" t="s">
         <v>26</v>
       </c>
       <c r="N26">
-        <v>4.8496</v>
+        <v>4.951</v>
       </c>
       <c r="S26" t="s">
         <v>26</v>
       </c>
       <c r="T26">
-        <v>4.8981</v>
+        <v>4.9995</v>
       </c>
       <c r="Y26" t="s">
         <v>26</v>
       </c>
       <c r="Z26">
-        <v>4.9123</v>
+        <v>5.0124</v>
       </c>
       <c r="AE26" t="s">
         <v>26</v>
       </c>
       <c r="AF26">
-        <v>4.9152</v>
+        <v>5.015</v>
       </c>
       <c r="AK26" t="s">
         <v>26</v>
       </c>
       <c r="AL26">
-        <v>4.915</v>
+        <v>5.015</v>
       </c>
       <c r="AQ26" t="s">
         <v>26</v>
       </c>
       <c r="AR26">
-        <v>4.9156</v>
+        <v>5.0148</v>
       </c>
       <c r="AW26" t="s">
         <v>26</v>
       </c>
       <c r="AX26">
-        <v>4.9161</v>
+        <v>5.0148</v>
       </c>
       <c r="BC26" t="s">
         <v>26</v>
       </c>
       <c r="BD26">
-        <v>4.9156</v>
+        <v>5.0149</v>
       </c>
     </row>
     <row r="27" spans="7:57">
@@ -2272,55 +2272,55 @@
         <v>27</v>
       </c>
       <c r="H27">
-        <v>-0.0019</v>
+        <v>0.0277</v>
       </c>
       <c r="M27" t="s">
         <v>27</v>
       </c>
       <c r="N27">
-        <v>-0.0455</v>
+        <v>0.0112</v>
       </c>
       <c r="S27" t="s">
         <v>27</v>
       </c>
       <c r="T27">
-        <v>-0.0039</v>
+        <v>0.0161</v>
       </c>
       <c r="Y27" t="s">
         <v>27</v>
       </c>
       <c r="Z27">
-        <v>-0.0219</v>
+        <v>0.0217</v>
       </c>
       <c r="AE27" t="s">
         <v>27</v>
       </c>
       <c r="AF27">
-        <v>0.0106</v>
+        <v>0.0219</v>
       </c>
       <c r="AK27" t="s">
         <v>27</v>
       </c>
       <c r="AL27">
-        <v>-0.0175</v>
+        <v>0.0218</v>
       </c>
       <c r="AQ27" t="s">
         <v>27</v>
       </c>
       <c r="AR27">
-        <v>0.0123</v>
+        <v>0.0218</v>
       </c>
       <c r="AW27" t="s">
         <v>27</v>
       </c>
       <c r="AX27">
-        <v>0.0007</v>
+        <v>0.0218</v>
       </c>
       <c r="BC27" t="s">
         <v>27</v>
       </c>
       <c r="BD27">
-        <v>0.0139</v>
+        <v>0.0218</v>
       </c>
     </row>
     <row r="28" spans="7:57">
@@ -2328,55 +2328,55 @@
         <v>28</v>
       </c>
       <c r="H28">
-        <v>0.7917999999999999</v>
+        <v>0.7966</v>
       </c>
       <c r="M28" t="s">
         <v>28</v>
       </c>
       <c r="N28">
-        <v>0.7212</v>
+        <v>0.7</v>
       </c>
       <c r="S28" t="s">
         <v>28</v>
       </c>
       <c r="T28">
-        <v>0.7308</v>
+        <v>0.7375</v>
       </c>
       <c r="Y28" t="s">
         <v>28</v>
       </c>
       <c r="Z28">
-        <v>0.7989000000000001</v>
+        <v>0.7998</v>
       </c>
       <c r="AE28" t="s">
         <v>28</v>
       </c>
       <c r="AF28">
-        <v>0.7994</v>
+        <v>0.7992</v>
       </c>
       <c r="AK28" t="s">
         <v>28</v>
       </c>
       <c r="AL28">
-        <v>0.7994</v>
+        <v>0.7992</v>
       </c>
       <c r="AQ28" t="s">
         <v>28</v>
       </c>
       <c r="AR28">
-        <v>0.7994</v>
+        <v>0.7992</v>
       </c>
       <c r="AW28" t="s">
         <v>28</v>
       </c>
       <c r="AX28">
-        <v>0.7994</v>
+        <v>0.7992</v>
       </c>
       <c r="BC28" t="s">
         <v>28</v>
       </c>
       <c r="BD28">
-        <v>0.7994</v>
+        <v>0.7992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>